<commit_message>
added tool to label data and upload improved dataset
</commit_message>
<xml_diff>
--- a/handwritten-math-expressions-dataset/Maths_eqations_handwritten.xlsx
+++ b/handwritten-math-expressions-dataset/Maths_eqations_handwritten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\downq\PycharmProjects\MISS\handwritten-math-expressions-dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5EDAD0-850C-428A-8EB0-7141BDD0BDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C10BC8-A6C6-44FC-B646-1060C08BE2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{2775A5C4-5C97-4141-B29B-DA96932C3D46}"/>
+    <workbookView xWindow="28575" yWindow="3120" windowWidth="38700" windowHeight="15345" xr2:uid="{2775A5C4-5C97-4141-B29B-DA96932C3D46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Expression</t>
   </si>
@@ -212,22 +212,25 @@
     <t>9 * 9 - 20</t>
   </si>
   <si>
-    <t>200 ÷ 50 + 8</t>
-  </si>
-  <si>
     <t>(10 * 2 ) - (3 * 4)</t>
   </si>
   <si>
-    <t>(9 + 1) - (9 - 1)</t>
-  </si>
-  <si>
     <t>4 * (3 + 5) - 7</t>
   </si>
   <si>
     <t>8 * (7 - 3)</t>
   </si>
   <si>
-    <t>(8 - 3) * 4</t>
+    <t>(25 - 3) * 2</t>
+  </si>
+  <si>
+    <t>20 ÷ 50 + 8</t>
+  </si>
+  <si>
+    <t>(18 - 3) * 4</t>
+  </si>
+  <si>
+    <t>(9 + 1) * (9 - 1)</t>
   </si>
 </sst>
 </file>
@@ -290,9 +293,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -330,7 +333,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -436,7 +439,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -578,7 +581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -586,19 +589,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D000-1140-4231-9E6A-8656603CEBFC}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="N67" sqref="N67"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -614,7 +617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -622,7 +625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -630,7 +633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -638,7 +641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -646,7 +649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -654,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -662,7 +665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -670,7 +673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -678,7 +681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -686,7 +689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -694,7 +697,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -702,7 +705,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -710,7 +713,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -718,7 +721,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -726,7 +729,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -734,7 +737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -742,7 +745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -750,7 +753,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -758,7 +761,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -766,7 +769,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -774,7 +777,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -782,7 +785,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -790,7 +793,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -798,7 +801,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -806,7 +809,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -814,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -822,7 +825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -830,7 +833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -838,7 +841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -846,7 +849,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -854,7 +857,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -862,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -870,7 +873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -878,203 +881,205 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>0.8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>1.3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>5.6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>8.4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>60</v>
       </c>
-      <c r="B55">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="B56">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="B58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>56</v>
       </c>
-      <c r="B57">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="B60">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>57</v>
       </c>
-      <c r="B58">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60">
+      <c r="B61">
         <v>40</v>
       </c>
     </row>

</xml_diff>